<commit_message>
Added generations data to pollinator requirements
</commit_message>
<xml_diff>
--- a/Pollinator_requirements.xlsx
+++ b/Pollinator_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CFA560-BE29-D74C-BD5B-387B3446C412}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C858045D-A011-7A47-B062-80809C56AF81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3558,10 +3558,10 @@
   <dimension ref="A1:DQ96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
change to nesting data for b. pascuorum and m. willughbiella
</commit_message>
<xml_diff>
--- a/Pollinator_requirements.xlsx
+++ b/Pollinator_requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16930A58-228C-184F-9C51-D30EDD16ED62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CFA04C-F0B5-114A-A4FA-F8DDF56D0377}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Species List" sheetId="2" r:id="rId1"/>
@@ -1383,7 +1383,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="422">
   <si>
     <t>Reliance</t>
   </si>
@@ -3098,14 +3098,14 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3570,10 +3570,10 @@
   <dimension ref="A1:DS111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AF76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AC38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AO97" sqref="AO97"/>
+      <selection pane="bottomRight" activeCell="AL51" sqref="AL51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7985,9 +7985,9 @@
       <c r="Y21" s="5">
         <v>1</v>
       </c>
-      <c r="Z21" s="48"/>
+      <c r="Z21" s="46"/>
       <c r="AA21" s="5"/>
-      <c r="AB21" s="48">
+      <c r="AB21" s="46">
         <v>1</v>
       </c>
       <c r="AC21" s="5"/>
@@ -10461,11 +10461,11 @@
       <c r="Y33" s="5">
         <v>1</v>
       </c>
-      <c r="Z33" s="48">
+      <c r="Z33" s="46">
         <v>1</v>
       </c>
       <c r="AA33" s="5"/>
-      <c r="AB33" s="48"/>
+      <c r="AB33" s="46"/>
       <c r="AC33" s="5"/>
       <c r="AD33" s="5"/>
       <c r="AE33" s="5"/>
@@ -12833,8 +12833,8 @@
       <c r="AC44" s="26"/>
       <c r="AF44" s="36"/>
       <c r="AG44" s="36"/>
-      <c r="AH44" s="5">
-        <v>0</v>
+      <c r="AH44" s="46">
+        <v>1</v>
       </c>
       <c r="AI44" s="5">
         <v>0</v>
@@ -17798,11 +17798,11 @@
       <c r="Y68" s="5">
         <v>1</v>
       </c>
-      <c r="Z68" s="48">
+      <c r="Z68" s="46">
         <v>1</v>
       </c>
       <c r="AA68" s="5"/>
-      <c r="AB68" s="48"/>
+      <c r="AB68" s="46"/>
       <c r="AC68" s="5"/>
       <c r="AD68" s="5"/>
       <c r="AE68" s="5"/>
@@ -20788,11 +20788,11 @@
       <c r="Z82" s="5">
         <v>1</v>
       </c>
-      <c r="AA82" s="48">
-        <v>1</v>
-      </c>
-      <c r="AB82" s="48"/>
-      <c r="AC82" s="48"/>
+      <c r="AA82" s="46">
+        <v>1</v>
+      </c>
+      <c r="AB82" s="46"/>
+      <c r="AC82" s="46"/>
       <c r="AD82" s="5"/>
       <c r="AE82" s="5"/>
       <c r="AF82" s="36"/>
@@ -22333,8 +22333,8 @@
       <c r="AR89" s="5">
         <v>0</v>
       </c>
-      <c r="AS89" s="5">
-        <v>0</v>
+      <c r="AS89" s="46">
+        <v>1</v>
       </c>
       <c r="AT89" s="5">
         <v>0</v>
@@ -23295,11 +23295,11 @@
       <c r="Y94" s="5">
         <v>1</v>
       </c>
-      <c r="Z94" s="48">
+      <c r="Z94" s="46">
         <v>1</v>
       </c>
       <c r="AA94" s="5"/>
-      <c r="AB94" s="48"/>
+      <c r="AB94" s="46"/>
       <c r="AC94" s="5"/>
       <c r="AD94" s="5"/>
       <c r="AE94" s="5"/>
@@ -23967,11 +23967,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2B0D57-B714-8B46-AC18-E8DEFB999C5C}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="21" customHeight="1"/>
@@ -23999,7 +23999,7 @@
       <c r="B2" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="47" t="s">
         <v>397</v>
       </c>
     </row>
@@ -24010,7 +24010,7 @@
       <c r="B3" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="46"/>
+      <c r="C3" s="47"/>
     </row>
     <row r="4" spans="1:3" ht="21" customHeight="1">
       <c r="A4" s="13" t="s">
@@ -24019,7 +24019,7 @@
       <c r="B4" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="46"/>
+      <c r="C4" s="47"/>
     </row>
     <row r="5" spans="1:3" ht="21" customHeight="1">
       <c r="A5" s="14" t="s">
@@ -24028,7 +24028,7 @@
       <c r="B5" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C5" s="46"/>
+      <c r="C5" s="47"/>
     </row>
     <row r="6" spans="1:3" ht="21" customHeight="1">
       <c r="A6" s="13" t="s">
@@ -24037,7 +24037,7 @@
       <c r="B6" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="47" t="s">
         <v>395</v>
       </c>
     </row>
@@ -24048,7 +24048,7 @@
       <c r="B7" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C7" s="46"/>
+      <c r="C7" s="47"/>
     </row>
     <row r="8" spans="1:3" ht="21" customHeight="1">
       <c r="A8" s="13" t="s">
@@ -24057,7 +24057,7 @@
       <c r="B8" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="47"/>
     </row>
     <row r="9" spans="1:3" ht="21" customHeight="1">
       <c r="A9" s="13" t="s">
@@ -24066,7 +24066,7 @@
       <c r="B9" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="47"/>
     </row>
     <row r="10" spans="1:3" ht="21" customHeight="1">
       <c r="A10" s="13" t="s">
@@ -24075,7 +24075,7 @@
       <c r="B10" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="47"/>
     </row>
     <row r="11" spans="1:3" ht="21" customHeight="1">
       <c r="A11" s="13" t="s">
@@ -24084,7 +24084,7 @@
       <c r="B11" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="47"/>
     </row>
     <row r="12" spans="1:3" ht="21" customHeight="1">
       <c r="A12" s="13" t="s">
@@ -24093,7 +24093,7 @@
       <c r="B12" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="47"/>
     </row>
     <row r="13" spans="1:3" ht="21" customHeight="1">
       <c r="A13" s="13" t="s">
@@ -24102,7 +24102,7 @@
       <c r="B13" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="47"/>
     </row>
     <row r="14" spans="1:3" ht="21" customHeight="1">
       <c r="A14" s="13" t="s">
@@ -24111,7 +24111,7 @@
       <c r="B14" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="47"/>
     </row>
     <row r="15" spans="1:3" ht="21" customHeight="1">
       <c r="A15" s="13" t="s">
@@ -24120,7 +24120,7 @@
       <c r="B15" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="C15" s="46"/>
+      <c r="C15" s="47"/>
     </row>
     <row r="16" spans="1:3" ht="21" customHeight="1">
       <c r="A16" s="13" t="s">
@@ -24129,7 +24129,7 @@
       <c r="B16" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C16" s="46"/>
+      <c r="C16" s="47"/>
     </row>
     <row r="17" spans="1:3" ht="21" customHeight="1">
       <c r="A17" s="13" t="s">
@@ -24138,7 +24138,7 @@
       <c r="B17" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C17" s="46"/>
+      <c r="C17" s="47"/>
     </row>
     <row r="18" spans="1:3" ht="21" customHeight="1">
       <c r="A18" s="13" t="s">
@@ -24147,7 +24147,7 @@
       <c r="B18" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="48" t="s">
         <v>394</v>
       </c>
     </row>
@@ -24158,7 +24158,7 @@
       <c r="B19" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="47"/>
+      <c r="C19" s="48"/>
     </row>
     <row r="20" spans="1:3" ht="21" customHeight="1">
       <c r="A20" s="14" t="s">
@@ -24167,7 +24167,7 @@
       <c r="B20" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C20" s="47"/>
+      <c r="C20" s="48"/>
     </row>
     <row r="21" spans="1:3" ht="21" customHeight="1">
       <c r="A21" s="13" t="s">
@@ -24176,7 +24176,7 @@
       <c r="B21" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C21" s="47"/>
+      <c r="C21" s="48"/>
     </row>
     <row r="22" spans="1:3" ht="21" customHeight="1">
       <c r="A22" s="13" t="s">
@@ -24185,7 +24185,7 @@
       <c r="B22" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C22" s="47"/>
+      <c r="C22" s="48"/>
     </row>
     <row r="23" spans="1:3" ht="21" customHeight="1">
       <c r="A23" s="13" t="s">
@@ -24194,7 +24194,7 @@
       <c r="B23" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="47"/>
+      <c r="C23" s="48"/>
     </row>
     <row r="24" spans="1:3" ht="21" customHeight="1">
       <c r="A24" s="14" t="s">
@@ -24203,97 +24203,115 @@
       <c r="B24" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C24" s="47"/>
+      <c r="C24" s="48"/>
     </row>
     <row r="25" spans="1:3" ht="21" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>24</v>
+        <v>421</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C25" s="47"/>
+        <v>197</v>
+      </c>
+      <c r="C25" s="48"/>
     </row>
     <row r="26" spans="1:3" ht="21" customHeight="1">
-      <c r="A26" s="13" t="s">
-        <v>25</v>
+      <c r="A26" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C26" s="47"/>
+        <v>198</v>
+      </c>
+      <c r="C26" s="48"/>
     </row>
     <row r="27" spans="1:3" ht="21" customHeight="1">
       <c r="A27" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C27" s="47"/>
+      <c r="C27" s="48"/>
     </row>
     <row r="28" spans="1:3" ht="21" customHeight="1">
       <c r="A28" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C28" s="47"/>
+      <c r="C28" s="48"/>
     </row>
     <row r="29" spans="1:3" ht="21" customHeight="1">
-      <c r="A29" s="14" t="s">
-        <v>28</v>
+      <c r="A29" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C29" s="47"/>
+      <c r="C29" s="48"/>
     </row>
     <row r="30" spans="1:3" ht="21" customHeight="1">
       <c r="A30" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="C30" s="46" t="s">
-        <v>396</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="C30" s="48"/>
     </row>
     <row r="31" spans="1:3" ht="21" customHeight="1">
       <c r="A31" s="14" t="s">
-        <v>30</v>
+        <v>420</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C31" s="46"/>
+        <v>212</v>
+      </c>
+      <c r="C31" s="48"/>
     </row>
     <row r="32" spans="1:3" ht="21" customHeight="1">
       <c r="A32" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="C32" s="46"/>
+        <v>199</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="21" customHeight="1">
       <c r="A33" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33" s="47"/>
+    </row>
+    <row r="34" spans="1:3" ht="21" customHeight="1">
+      <c r="A34" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C34" s="47"/>
+    </row>
+    <row r="35" spans="1:3" ht="21" customHeight="1">
+      <c r="A35" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B35" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C33" s="46"/>
+      <c r="C35" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C17"/>
-    <mergeCell ref="C18:C29"/>
-    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="C18:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>